<commit_message>
[minor] missing files investigation
</commit_message>
<xml_diff>
--- a/datasets/glider/meta/missing_labels.xlsx
+++ b/datasets/glider/meta/missing_labels.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="2817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="2817">
   <si>
     <t>source_file</t>
   </si>
@@ -8827,7 +8827,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10309,16 +10309,16 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D74" s="2">
-        <v>43305.00833333333</v>
+        <v>43303.79305555556</v>
       </c>
       <c r="E74" s="2">
-        <v>43305.00902777778</v>
+        <v>43303.80902777778</v>
       </c>
       <c r="F74" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -10329,16 +10329,16 @@
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D75" s="2">
-        <v>43308.68402777778</v>
+        <v>43303.92361111111</v>
       </c>
       <c r="E75" s="2">
-        <v>43308.69444444445</v>
+        <v>43303.94444444445</v>
       </c>
       <c r="F75" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -10349,16 +10349,16 @@
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D76" s="2">
-        <v>43308.71041666667</v>
+        <v>43304.01875</v>
       </c>
       <c r="E76" s="2">
-        <v>43308.74375</v>
+        <v>43304.02708333333</v>
       </c>
       <c r="F76" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -10369,16 +10369,16 @@
         <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D77" s="2">
-        <v>43308.78263888889</v>
+        <v>43304.05972222222</v>
       </c>
       <c r="E77" s="2">
-        <v>43308.8125</v>
+        <v>43304.06527777778</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -10386,19 +10386,19 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D78" s="2">
-        <v>43310.6375</v>
+        <v>43304.24861111111</v>
       </c>
       <c r="E78" s="2">
-        <v>43310.63958333333</v>
+        <v>43304.25486111111</v>
       </c>
       <c r="F78" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -10406,16 +10406,16 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D79" s="2">
-        <v>43310.68055555555</v>
+        <v>43304.27916666667</v>
       </c>
       <c r="E79" s="2">
-        <v>43310.68125</v>
+        <v>43304.3</v>
       </c>
       <c r="F79" t="s">
         <v>108</v>
@@ -10426,19 +10426,19 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D80" s="2">
-        <v>43311.69791666666</v>
+        <v>43304.41944444444</v>
       </c>
       <c r="E80" s="2">
-        <v>43311.69861111111</v>
+        <v>43304.43611111111</v>
       </c>
       <c r="F80" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -10446,16 +10446,16 @@
         <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D81" s="2">
-        <v>43311.74236111111</v>
+        <v>43304.45694444444</v>
       </c>
       <c r="E81" s="2">
-        <v>43311.75347222222</v>
+        <v>43304.475</v>
       </c>
       <c r="F81" t="s">
         <v>108</v>
@@ -10466,16 +10466,16 @@
         <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D82" s="2">
-        <v>43311.74375</v>
+        <v>43304.45972222222</v>
       </c>
       <c r="E82" s="2">
-        <v>43311.74513888889</v>
+        <v>43304.47291666667</v>
       </c>
       <c r="F82" t="s">
         <v>108</v>
@@ -10486,19 +10486,19 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D83" s="2">
-        <v>43311.91111111111</v>
+        <v>43304.64652777778</v>
       </c>
       <c r="E83" s="2">
-        <v>43311.91180555556</v>
+        <v>43304.64930555555</v>
       </c>
       <c r="F83" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -10506,16 +10506,16 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D84" s="2">
-        <v>43312.05625</v>
+        <v>43304.80972222222</v>
       </c>
       <c r="E84" s="2">
-        <v>43312.0625</v>
+        <v>43304.81597222222</v>
       </c>
       <c r="F84" t="s">
         <v>108</v>
@@ -10526,19 +10526,19 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D85" s="2">
-        <v>43312.79513888889</v>
+        <v>43304.89861111111</v>
       </c>
       <c r="E85" s="2">
-        <v>43312.8</v>
+        <v>43304.91944444444</v>
       </c>
       <c r="F85" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -10546,19 +10546,19 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D86" s="2">
-        <v>43312.86180555556</v>
+        <v>43305.10069444445</v>
       </c>
       <c r="E86" s="2">
-        <v>43312.8625</v>
+        <v>43305.12291666667</v>
       </c>
       <c r="F86" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -10566,16 +10566,16 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D87" s="2">
-        <v>43312.89861111111</v>
+        <v>43305.26666666667</v>
       </c>
       <c r="E87" s="2">
-        <v>43312.90555555555</v>
+        <v>43305.28402777778</v>
       </c>
       <c r="F87" t="s">
         <v>108</v>
@@ -10586,19 +10586,19 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D88" s="2">
-        <v>43314.19861111111</v>
+        <v>43305.66597222222</v>
       </c>
       <c r="E88" s="2">
-        <v>43314.20277777778</v>
+        <v>43305.68472222222</v>
       </c>
       <c r="F88" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -10606,16 +10606,16 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="C89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D89" s="2">
-        <v>43314.30972222222</v>
+        <v>43306.60555555556</v>
       </c>
       <c r="E89" s="2">
-        <v>43314.31111111111</v>
+        <v>43306.62013888889</v>
       </c>
       <c r="F89" t="s">
         <v>108</v>
@@ -10626,19 +10626,19 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D90" s="2">
-        <v>43314.3125</v>
+        <v>43306.65486111111</v>
       </c>
       <c r="E90" s="2">
-        <v>43314.31319444445</v>
+        <v>43306.66388888889</v>
       </c>
       <c r="F90" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -10646,19 +10646,19 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D91" s="2">
-        <v>43317.33888888889</v>
+        <v>43307.1</v>
       </c>
       <c r="E91" s="2">
-        <v>43317.35347222222</v>
+        <v>43307.10416666666</v>
       </c>
       <c r="F91" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -10666,19 +10666,19 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D92" s="2">
-        <v>43317.36944444444</v>
+        <v>43307.41458333333</v>
       </c>
       <c r="E92" s="2">
-        <v>43317.37152777778</v>
+        <v>43307.43125</v>
       </c>
       <c r="F92" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -10686,19 +10686,19 @@
         <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D93" s="2">
-        <v>43319.05486111111</v>
+        <v>43308.13541666666</v>
       </c>
       <c r="E93" s="2">
-        <v>43319.05555555555</v>
+        <v>43308.15833333333</v>
       </c>
       <c r="F93" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -10706,19 +10706,19 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D94" s="2">
-        <v>43320.06597222222</v>
+        <v>43308.84930555556</v>
       </c>
       <c r="E94" s="2">
-        <v>43320.06805555556</v>
+        <v>43308.85972222222</v>
       </c>
       <c r="F94" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -10726,19 +10726,19 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D95" s="2">
-        <v>43320.11875</v>
+        <v>43309.40694444445</v>
       </c>
       <c r="E95" s="2">
-        <v>43320.11944444444</v>
+        <v>43309.41944444444</v>
       </c>
       <c r="F95" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -10746,19 +10746,19 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D96" s="2">
-        <v>43320.57708333333</v>
+        <v>43309.98194444444</v>
       </c>
       <c r="E96" s="2">
-        <v>43320.57916666667</v>
+        <v>43309.00208333333</v>
       </c>
       <c r="F96" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -10766,19 +10766,19 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D97" s="2">
-        <v>43320.60069444445</v>
+        <v>43310.81805555556</v>
       </c>
       <c r="E97" s="2">
-        <v>43320.60138888889</v>
+        <v>43310.83055555556</v>
       </c>
       <c r="F97" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -10786,19 +10786,19 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D98" s="2">
-        <v>43320.63125</v>
+        <v>43310.82430555556</v>
       </c>
       <c r="E98" s="2">
-        <v>43320.63680555556</v>
+        <v>43310.82986111111</v>
       </c>
       <c r="F98" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -10806,19 +10806,19 @@
         <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D99" s="2">
-        <v>43320.84444444445</v>
+        <v>43311.98819444444</v>
       </c>
       <c r="E99" s="2">
-        <v>43320.84861111111</v>
+        <v>43311.98888888889</v>
       </c>
       <c r="F99" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -10826,19 +10826,19 @@
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D100" s="2">
-        <v>43326.50625</v>
+        <v>43313.46527777778</v>
       </c>
       <c r="E100" s="2">
-        <v>43326.50694444445</v>
+        <v>43313.475</v>
       </c>
       <c r="F100" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -10846,19 +10846,19 @@
         <v>6</v>
       </c>
       <c r="B101" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D101" s="2">
-        <v>43327.34444444445</v>
+        <v>43313.86458333334</v>
       </c>
       <c r="E101" s="2">
-        <v>43327.34513888889</v>
+        <v>43313.86666666667</v>
       </c>
       <c r="F101" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -10866,19 +10866,19 @@
         <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="C102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D102" s="2">
-        <v>43327.35347222222</v>
+        <v>43313.93333333333</v>
       </c>
       <c r="E102" s="2">
-        <v>43327.36388888889</v>
+        <v>43313.93402777778</v>
       </c>
       <c r="F102" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -10886,19 +10886,19 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="C103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D103" s="2">
-        <v>43339.225</v>
+        <v>43313.93611111111</v>
       </c>
       <c r="E103" s="2">
-        <v>43339.22569444445</v>
+        <v>43313.93680555555</v>
       </c>
       <c r="F103" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -10906,378 +10906,1498 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="C104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D104" s="2">
-        <v>43339.45833333334</v>
+        <v>43315.35833333333</v>
       </c>
       <c r="E104" s="2">
-        <v>43339.45902777778</v>
+        <v>43315.36944444444</v>
       </c>
       <c r="F104" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C105" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D105" s="2">
-        <v>43316.28333333333</v>
+        <v>43315.56875</v>
       </c>
       <c r="E105" s="2">
-        <v>43316.29236111111</v>
+        <v>43315.57361111111</v>
       </c>
       <c r="F105" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C106" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D106" s="2">
-        <v>43317.55486111111</v>
+        <v>43320.27847222222</v>
       </c>
       <c r="E106" s="2">
-        <v>43317.56527777778</v>
+        <v>43320.28541666667</v>
       </c>
       <c r="F106" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C107" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D107" s="2">
-        <v>43317.71527777778</v>
+        <v>43320.58611111111</v>
       </c>
       <c r="E107" s="2">
-        <v>43317.72291666667</v>
+        <v>43320.59236111111</v>
       </c>
       <c r="F107" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D108" s="2">
-        <v>43319.60277777778</v>
+        <v>43322.25347222222</v>
       </c>
       <c r="E108" s="2">
-        <v>43319.60763888889</v>
+        <v>43322.26041666666</v>
       </c>
       <c r="F108" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D109" s="2">
-        <v>43319.82222222222</v>
+        <v>43322.38194444445</v>
       </c>
       <c r="E109" s="2">
-        <v>43319.82916666667</v>
+        <v>43322.38819444444</v>
       </c>
       <c r="F109" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D110" s="2">
-        <v>43319.89305555556</v>
+        <v>43326.84166666667</v>
       </c>
       <c r="E110" s="2">
-        <v>43319.9</v>
+        <v>43326.84236111111</v>
       </c>
       <c r="F110" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C111" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D111" s="2">
-        <v>43319.94166666667</v>
+        <v>43327.22708333333</v>
       </c>
       <c r="E111" s="2">
-        <v>43319.94305555556</v>
+        <v>43327.23611111111</v>
       </c>
       <c r="F111" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D112" s="2">
-        <v>43320.0125</v>
+        <v>43327.99930555555</v>
       </c>
       <c r="E112" s="2">
-        <v>43320.01736111111</v>
+        <v>43327.01736111111</v>
       </c>
       <c r="F112" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D113" s="2">
-        <v>43325.30694444444</v>
+        <v>43329.69791666666</v>
       </c>
       <c r="E113" s="2">
-        <v>43325.31180555555</v>
+        <v>43329.70138888889</v>
       </c>
       <c r="F113" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D114" s="2">
-        <v>43326.29375</v>
+        <v>43329.97708333333</v>
       </c>
       <c r="E114" s="2">
-        <v>43326.3</v>
+        <v>43329.97916666666</v>
       </c>
       <c r="F114" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C115" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D115" s="2">
-        <v>43327.36458333334</v>
+        <v>43330.23125</v>
       </c>
       <c r="E115" s="2">
-        <v>43327.36597222222</v>
+        <v>43330.23194444444</v>
       </c>
       <c r="F115" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D116" s="2">
-        <v>43327.99652777778</v>
+        <v>43330.25069444445</v>
       </c>
       <c r="E116" s="2">
-        <v>43327.99930555555</v>
+        <v>43330.25486111111</v>
       </c>
       <c r="F116" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C117" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D117" s="2">
-        <v>43328.77430555555</v>
+        <v>43333.50555555556</v>
       </c>
       <c r="E117" s="2">
-        <v>43328.78055555555</v>
+        <v>43333.50625</v>
       </c>
       <c r="F117" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C118" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D118" s="2">
-        <v>43329.15486111111</v>
+        <v>43333.76458333333</v>
       </c>
       <c r="E118" s="2">
-        <v>43329.16666666666</v>
+        <v>43333.77083333334</v>
       </c>
       <c r="F118" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C119" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D119" s="2">
-        <v>43337.35763888889</v>
+        <v>43333.98472222222</v>
       </c>
       <c r="E119" s="2">
-        <v>43337.36180555556</v>
+        <v>43333.02152777778</v>
       </c>
       <c r="F119" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C120" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D120" s="2">
-        <v>43340.09930555556</v>
+        <v>43336.28263888889</v>
       </c>
       <c r="E120" s="2">
-        <v>43340.10625</v>
+        <v>43336.28958333333</v>
       </c>
       <c r="F120" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C121" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D121" s="2">
-        <v>43341.70138888889</v>
+        <v>43338.02708333333</v>
       </c>
       <c r="E121" s="2">
-        <v>43341.70347222222</v>
+        <v>43338.0375</v>
       </c>
       <c r="F121" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
+        <v>6</v>
+      </c>
+      <c r="B122" t="s">
+        <v>76</v>
+      </c>
+      <c r="C122" t="s">
+        <v>105</v>
+      </c>
+      <c r="D122" s="2">
+        <v>43338.97152777778</v>
+      </c>
+      <c r="E122" s="2">
+        <v>43338.975</v>
+      </c>
+      <c r="F122" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" t="s">
+        <v>105</v>
+      </c>
+      <c r="D123" s="2">
+        <v>43340.98263888889</v>
+      </c>
+      <c r="E123" s="2">
+        <v>43340.02013888889</v>
+      </c>
+      <c r="F123" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" t="s">
+        <v>105</v>
+      </c>
+      <c r="D124" s="2">
+        <v>43342.00902777778</v>
+      </c>
+      <c r="E124" s="2">
+        <v>43342.01319444444</v>
+      </c>
+      <c r="F124" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" t="s">
+        <v>79</v>
+      </c>
+      <c r="C125" t="s">
+        <v>105</v>
+      </c>
+      <c r="D125" s="2">
+        <v>43342.6125</v>
+      </c>
+      <c r="E125" s="2">
+        <v>43342.6375</v>
+      </c>
+      <c r="F125" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" t="s">
+        <v>106</v>
+      </c>
+      <c r="D126" s="2">
+        <v>43305.00833333333</v>
+      </c>
+      <c r="E126" s="2">
+        <v>43305.00902777778</v>
+      </c>
+      <c r="F126" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" t="s">
+        <v>106</v>
+      </c>
+      <c r="D127" s="2">
+        <v>43308.68402777778</v>
+      </c>
+      <c r="E127" s="2">
+        <v>43308.69444444445</v>
+      </c>
+      <c r="F127" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>6</v>
+      </c>
+      <c r="B128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" t="s">
+        <v>106</v>
+      </c>
+      <c r="D128" s="2">
+        <v>43308.71041666667</v>
+      </c>
+      <c r="E128" s="2">
+        <v>43308.74375</v>
+      </c>
+      <c r="F128" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" t="s">
+        <v>106</v>
+      </c>
+      <c r="D129" s="2">
+        <v>43308.78263888889</v>
+      </c>
+      <c r="E129" s="2">
+        <v>43308.8125</v>
+      </c>
+      <c r="F129" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>6</v>
+      </c>
+      <c r="B130" t="s">
+        <v>13</v>
+      </c>
+      <c r="C130" t="s">
+        <v>106</v>
+      </c>
+      <c r="D130" s="2">
+        <v>43310.6375</v>
+      </c>
+      <c r="E130" s="2">
+        <v>43310.63958333333</v>
+      </c>
+      <c r="F130" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131" t="s">
+        <v>106</v>
+      </c>
+      <c r="D131" s="2">
+        <v>43310.68055555555</v>
+      </c>
+      <c r="E131" s="2">
+        <v>43310.68125</v>
+      </c>
+      <c r="F131" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" t="s">
+        <v>106</v>
+      </c>
+      <c r="D132" s="2">
+        <v>43311.69791666666</v>
+      </c>
+      <c r="E132" s="2">
+        <v>43311.69861111111</v>
+      </c>
+      <c r="F132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>6</v>
+      </c>
+      <c r="B133" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" t="s">
+        <v>106</v>
+      </c>
+      <c r="D133" s="2">
+        <v>43311.74236111111</v>
+      </c>
+      <c r="E133" s="2">
+        <v>43311.75347222222</v>
+      </c>
+      <c r="F133" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" t="s">
+        <v>106</v>
+      </c>
+      <c r="D134" s="2">
+        <v>43311.74375</v>
+      </c>
+      <c r="E134" s="2">
+        <v>43311.74513888889</v>
+      </c>
+      <c r="F134" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" t="s">
+        <v>106</v>
+      </c>
+      <c r="D135" s="2">
+        <v>43311.91111111111</v>
+      </c>
+      <c r="E135" s="2">
+        <v>43311.91180555556</v>
+      </c>
+      <c r="F135" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" t="s">
+        <v>26</v>
+      </c>
+      <c r="C136" t="s">
+        <v>106</v>
+      </c>
+      <c r="D136" s="2">
+        <v>43312.05625</v>
+      </c>
+      <c r="E136" s="2">
+        <v>43312.0625</v>
+      </c>
+      <c r="F136" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" t="s">
+        <v>33</v>
+      </c>
+      <c r="C137" t="s">
+        <v>106</v>
+      </c>
+      <c r="D137" s="2">
+        <v>43312.79513888889</v>
+      </c>
+      <c r="E137" s="2">
+        <v>43312.8</v>
+      </c>
+      <c r="F137" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" t="s">
+        <v>80</v>
+      </c>
+      <c r="C138" t="s">
+        <v>106</v>
+      </c>
+      <c r="D138" s="2">
+        <v>43312.86180555556</v>
+      </c>
+      <c r="E138" s="2">
+        <v>43312.8625</v>
+      </c>
+      <c r="F138" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>6</v>
+      </c>
+      <c r="B139" t="s">
+        <v>81</v>
+      </c>
+      <c r="C139" t="s">
+        <v>106</v>
+      </c>
+      <c r="D139" s="2">
+        <v>43312.89861111111</v>
+      </c>
+      <c r="E139" s="2">
+        <v>43312.90555555555</v>
+      </c>
+      <c r="F139" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>6</v>
+      </c>
+      <c r="B140" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" t="s">
+        <v>106</v>
+      </c>
+      <c r="D140" s="2">
+        <v>43314.19861111111</v>
+      </c>
+      <c r="E140" s="2">
+        <v>43314.20277777778</v>
+      </c>
+      <c r="F140" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+      <c r="C141" t="s">
+        <v>106</v>
+      </c>
+      <c r="D141" s="2">
+        <v>43314.30972222222</v>
+      </c>
+      <c r="E141" s="2">
+        <v>43314.31111111111</v>
+      </c>
+      <c r="F141" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" t="s">
+        <v>34</v>
+      </c>
+      <c r="C142" t="s">
+        <v>106</v>
+      </c>
+      <c r="D142" s="2">
+        <v>43314.3125</v>
+      </c>
+      <c r="E142" s="2">
+        <v>43314.31319444445</v>
+      </c>
+      <c r="F142" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" t="s">
+        <v>84</v>
+      </c>
+      <c r="C143" t="s">
+        <v>106</v>
+      </c>
+      <c r="D143" s="2">
+        <v>43317.33888888889</v>
+      </c>
+      <c r="E143" s="2">
+        <v>43317.35347222222</v>
+      </c>
+      <c r="F143" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s">
+        <v>85</v>
+      </c>
+      <c r="C144" t="s">
+        <v>106</v>
+      </c>
+      <c r="D144" s="2">
+        <v>43317.36944444444</v>
+      </c>
+      <c r="E144" s="2">
+        <v>43317.37152777778</v>
+      </c>
+      <c r="F144" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s">
+        <v>86</v>
+      </c>
+      <c r="C145" t="s">
+        <v>106</v>
+      </c>
+      <c r="D145" s="2">
+        <v>43319.05486111111</v>
+      </c>
+      <c r="E145" s="2">
+        <v>43319.05555555555</v>
+      </c>
+      <c r="F145" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" t="s">
+        <v>87</v>
+      </c>
+      <c r="C146" t="s">
+        <v>106</v>
+      </c>
+      <c r="D146" s="2">
+        <v>43320.06597222222</v>
+      </c>
+      <c r="E146" s="2">
+        <v>43320.06805555556</v>
+      </c>
+      <c r="F146" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" t="s">
+        <v>35</v>
+      </c>
+      <c r="C147" t="s">
+        <v>106</v>
+      </c>
+      <c r="D147" s="2">
+        <v>43320.11875</v>
+      </c>
+      <c r="E147" s="2">
+        <v>43320.11944444444</v>
+      </c>
+      <c r="F147" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s">
+        <v>88</v>
+      </c>
+      <c r="C148" t="s">
+        <v>106</v>
+      </c>
+      <c r="D148" s="2">
+        <v>43320.57708333333</v>
+      </c>
+      <c r="E148" s="2">
+        <v>43320.57916666667</v>
+      </c>
+      <c r="F148" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>89</v>
+      </c>
+      <c r="C149" t="s">
+        <v>106</v>
+      </c>
+      <c r="D149" s="2">
+        <v>43320.60069444445</v>
+      </c>
+      <c r="E149" s="2">
+        <v>43320.60138888889</v>
+      </c>
+      <c r="F149" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" t="s">
+        <v>90</v>
+      </c>
+      <c r="C150" t="s">
+        <v>106</v>
+      </c>
+      <c r="D150" s="2">
+        <v>43320.63125</v>
+      </c>
+      <c r="E150" s="2">
+        <v>43320.63680555556</v>
+      </c>
+      <c r="F150" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>91</v>
+      </c>
+      <c r="C151" t="s">
+        <v>106</v>
+      </c>
+      <c r="D151" s="2">
+        <v>43320.84444444445</v>
+      </c>
+      <c r="E151" s="2">
+        <v>43320.84861111111</v>
+      </c>
+      <c r="F151" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>6</v>
+      </c>
+      <c r="B152" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" t="s">
+        <v>106</v>
+      </c>
+      <c r="D152" s="2">
+        <v>43326.50625</v>
+      </c>
+      <c r="E152" s="2">
+        <v>43326.50694444445</v>
+      </c>
+      <c r="F152" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>6</v>
+      </c>
+      <c r="B153" t="s">
+        <v>92</v>
+      </c>
+      <c r="C153" t="s">
+        <v>106</v>
+      </c>
+      <c r="D153" s="2">
+        <v>43327.34444444445</v>
+      </c>
+      <c r="E153" s="2">
+        <v>43327.34513888889</v>
+      </c>
+      <c r="F153" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154" t="s">
+        <v>93</v>
+      </c>
+      <c r="C154" t="s">
+        <v>106</v>
+      </c>
+      <c r="D154" s="2">
+        <v>43327.35347222222</v>
+      </c>
+      <c r="E154" s="2">
+        <v>43327.36388888889</v>
+      </c>
+      <c r="F154" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" t="s">
+        <v>6</v>
+      </c>
+      <c r="B155" t="s">
+        <v>94</v>
+      </c>
+      <c r="C155" t="s">
+        <v>106</v>
+      </c>
+      <c r="D155" s="2">
+        <v>43339.225</v>
+      </c>
+      <c r="E155" s="2">
+        <v>43339.22569444445</v>
+      </c>
+      <c r="F155" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" t="s">
+        <v>95</v>
+      </c>
+      <c r="C156" t="s">
+        <v>106</v>
+      </c>
+      <c r="D156" s="2">
+        <v>43339.45833333334</v>
+      </c>
+      <c r="E156" s="2">
+        <v>43339.45902777778</v>
+      </c>
+      <c r="F156" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" t="s">
+        <v>6</v>
+      </c>
+      <c r="B157" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157" t="s">
+        <v>106</v>
+      </c>
+      <c r="D157" s="2">
+        <v>43308.68402777778</v>
+      </c>
+      <c r="E157" s="2">
+        <v>43308.69444444445</v>
+      </c>
+      <c r="F157" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" t="s">
+        <v>26</v>
+      </c>
+      <c r="C158" t="s">
+        <v>106</v>
+      </c>
+      <c r="D158" s="2">
+        <v>43312.05625</v>
+      </c>
+      <c r="E158" s="2">
+        <v>43312.0625</v>
+      </c>
+      <c r="F158" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" t="s">
+        <v>106</v>
+      </c>
+      <c r="D159" s="2">
+        <v>43314.19861111111</v>
+      </c>
+      <c r="E159" s="2">
+        <v>43314.20277777778</v>
+      </c>
+      <c r="F159" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160" t="s">
+        <v>83</v>
+      </c>
+      <c r="C160" t="s">
+        <v>106</v>
+      </c>
+      <c r="D160" s="2">
+        <v>43314.30972222222</v>
+      </c>
+      <c r="E160" s="2">
+        <v>43314.31111111111</v>
+      </c>
+      <c r="F160" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
         <v>7</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B161" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" t="s">
+        <v>107</v>
+      </c>
+      <c r="D161" s="2">
+        <v>43316.28333333333</v>
+      </c>
+      <c r="E161" s="2">
+        <v>43316.29236111111</v>
+      </c>
+      <c r="F161" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
+        <v>7</v>
+      </c>
+      <c r="B162" t="s">
+        <v>20</v>
+      </c>
+      <c r="C162" t="s">
+        <v>107</v>
+      </c>
+      <c r="D162" s="2">
+        <v>43317.55486111111</v>
+      </c>
+      <c r="E162" s="2">
+        <v>43317.56527777778</v>
+      </c>
+      <c r="F162" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>24</v>
+      </c>
+      <c r="C163" t="s">
+        <v>107</v>
+      </c>
+      <c r="D163" s="2">
+        <v>43317.71527777778</v>
+      </c>
+      <c r="E163" s="2">
+        <v>43317.72291666667</v>
+      </c>
+      <c r="F163" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" t="s">
+        <v>7</v>
+      </c>
+      <c r="B164" t="s">
+        <v>30</v>
+      </c>
+      <c r="C164" t="s">
+        <v>107</v>
+      </c>
+      <c r="D164" s="2">
+        <v>43319.60277777778</v>
+      </c>
+      <c r="E164" s="2">
+        <v>43319.60763888889</v>
+      </c>
+      <c r="F164" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165" t="s">
+        <v>96</v>
+      </c>
+      <c r="C165" t="s">
+        <v>107</v>
+      </c>
+      <c r="D165" s="2">
+        <v>43319.82222222222</v>
+      </c>
+      <c r="E165" s="2">
+        <v>43319.82916666667</v>
+      </c>
+      <c r="F165" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" t="s">
+        <v>97</v>
+      </c>
+      <c r="C166" t="s">
+        <v>107</v>
+      </c>
+      <c r="D166" s="2">
+        <v>43319.89305555556</v>
+      </c>
+      <c r="E166" s="2">
+        <v>43319.9</v>
+      </c>
+      <c r="F166" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" t="s">
+        <v>98</v>
+      </c>
+      <c r="C167" t="s">
+        <v>107</v>
+      </c>
+      <c r="D167" s="2">
+        <v>43319.94166666667</v>
+      </c>
+      <c r="E167" s="2">
+        <v>43319.94305555556</v>
+      </c>
+      <c r="F167" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" t="s">
+        <v>33</v>
+      </c>
+      <c r="C168" t="s">
+        <v>107</v>
+      </c>
+      <c r="D168" s="2">
+        <v>43320.0125</v>
+      </c>
+      <c r="E168" s="2">
+        <v>43320.01736111111</v>
+      </c>
+      <c r="F168" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" t="s">
+        <v>89</v>
+      </c>
+      <c r="C169" t="s">
+        <v>107</v>
+      </c>
+      <c r="D169" s="2">
+        <v>43325.30694444444</v>
+      </c>
+      <c r="E169" s="2">
+        <v>43325.31180555555</v>
+      </c>
+      <c r="F169" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" t="s">
+        <v>93</v>
+      </c>
+      <c r="C170" t="s">
+        <v>107</v>
+      </c>
+      <c r="D170" s="2">
+        <v>43326.29375</v>
+      </c>
+      <c r="E170" s="2">
+        <v>43326.3</v>
+      </c>
+      <c r="F170" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>99</v>
+      </c>
+      <c r="C171" t="s">
+        <v>107</v>
+      </c>
+      <c r="D171" s="2">
+        <v>43327.36458333334</v>
+      </c>
+      <c r="E171" s="2">
+        <v>43327.36597222222</v>
+      </c>
+      <c r="F171" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B172" t="s">
+        <v>100</v>
+      </c>
+      <c r="C172" t="s">
+        <v>107</v>
+      </c>
+      <c r="D172" s="2">
+        <v>43327.99652777778</v>
+      </c>
+      <c r="E172" s="2">
+        <v>43327.99930555555</v>
+      </c>
+      <c r="F172" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" t="s">
+        <v>7</v>
+      </c>
+      <c r="B173" t="s">
+        <v>101</v>
+      </c>
+      <c r="C173" t="s">
+        <v>107</v>
+      </c>
+      <c r="D173" s="2">
+        <v>43328.77430555555</v>
+      </c>
+      <c r="E173" s="2">
+        <v>43328.78055555555</v>
+      </c>
+      <c r="F173" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174" t="s">
+        <v>44</v>
+      </c>
+      <c r="C174" t="s">
+        <v>107</v>
+      </c>
+      <c r="D174" s="2">
+        <v>43329.15486111111</v>
+      </c>
+      <c r="E174" s="2">
+        <v>43329.16666666666</v>
+      </c>
+      <c r="F174" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" t="s">
+        <v>102</v>
+      </c>
+      <c r="C175" t="s">
+        <v>107</v>
+      </c>
+      <c r="D175" s="2">
+        <v>43337.35763888889</v>
+      </c>
+      <c r="E175" s="2">
+        <v>43337.36180555556</v>
+      </c>
+      <c r="F175" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" t="s">
+        <v>7</v>
+      </c>
+      <c r="B176" t="s">
+        <v>103</v>
+      </c>
+      <c r="C176" t="s">
+        <v>107</v>
+      </c>
+      <c r="D176" s="2">
+        <v>43340.09930555556</v>
+      </c>
+      <c r="E176" s="2">
+        <v>43340.10625</v>
+      </c>
+      <c r="F176" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177" t="s">
+        <v>104</v>
+      </c>
+      <c r="C177" t="s">
+        <v>107</v>
+      </c>
+      <c r="D177" s="2">
+        <v>43341.70138888889</v>
+      </c>
+      <c r="E177" s="2">
+        <v>43341.70347222222</v>
+      </c>
+      <c r="F177" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" t="s">
+        <v>7</v>
+      </c>
+      <c r="B178" t="s">
         <v>50</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C178" t="s">
         <v>107</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D178" s="2">
         <v>43342</v>
       </c>
-      <c r="E122" s="2">
+      <c r="E178" s="2">
         <v>43342.00902777778</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F178" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>